<commit_message>
Tool adjustments, applying the recommendations, modifying the analysis excel file, added comparison viewer for the changes.
</commit_message>
<xml_diff>
--- a/src/bpmn_analysis_results_v0.xlsx
+++ b/src/bpmn_analysis_results_v0.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Modelowanie biznesowe\LLM-BPMN-Checker\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E6790-A06B-4DA8-AA1B-0A0BDA71F8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E198C3-0C10-4A15-ADA6-55281BB7E457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26028" yWindow="-108" windowWidth="26136" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors (multiple)" sheetId="3" r:id="rId1"/>
     <sheet name="Errors (single)" sheetId="1" r:id="rId2"/>
     <sheet name="Stats" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Errors (single)'!$A$2:$K$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="295">
   <si>
     <t>elements</t>
   </si>
@@ -930,7 +933,22 @@
     <t>MULTIPLE</t>
   </si>
   <si>
-    <t>Could be done using tools?</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ORIGINAL Did LLM fix?</t>
+  </si>
+  <si>
+    <t>DETECTED Did LLM fix?</t>
+  </si>
+  <si>
+    <t>Ex</t>
+  </si>
+  <si>
+    <t>Err</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1016,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1026,6 +1044,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1174,7 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1203,15 +1227,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1224,13 +1239,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB51515"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1529,831 +1572,1201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE00482C-EF80-45B0-86A0-B6AC14D560E4}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="41.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="17.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="3" max="8" width="41.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="17.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="46.5703125" customWidth="1"/>
+    <col min="12" max="12" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="E1" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="G1" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="K1" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="E2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="G2" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="H2" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="G2" s="24">
+      <c r="I2" s="21">
         <v>3</v>
       </c>
-      <c r="H2" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="J2" s="21">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>289</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="F3" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="G3" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="H3" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G3" s="24">
+      <c r="I3" s="21">
         <v>10</v>
       </c>
-      <c r="H3" s="24">
+      <c r="J3" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="K3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="E4" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="F4" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="G4" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="H4" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G4" s="24">
+      <c r="I4" s="21">
         <v>10</v>
       </c>
-      <c r="H4" s="24">
+      <c r="J4" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="K4" t="s">
+        <v>289</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="E5" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="F5" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="G5" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="H5" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="24">
+      <c r="I5" s="21">
         <v>10</v>
       </c>
-      <c r="H5" s="24">
+      <c r="J5" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="K5" t="s">
+        <v>289</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="E6" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="F6" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="G6" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="H6" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="24">
+      <c r="I6" s="21">
         <v>3</v>
       </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="J6" s="21">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="E7" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="F7" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="G7" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="H7" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="G7" s="24">
+      <c r="I7" s="21">
         <v>3</v>
       </c>
-      <c r="H7" s="24">
+      <c r="J7" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="K7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="F8" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="G8" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="H8" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="G8" s="24">
+      <c r="I8" s="21">
         <v>10</v>
       </c>
-      <c r="H8" s="24">
+      <c r="J8" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="K8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="E9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="F9" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="G9" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="H9" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="G9" s="24">
+      <c r="I9" s="21">
         <v>9</v>
       </c>
-      <c r="H9" s="24">
+      <c r="J9" s="21">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="K9" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="F10" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="G10" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="H10" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="G10" s="24">
+      <c r="I10" s="21">
         <v>5</v>
       </c>
-      <c r="H10" s="24">
+      <c r="J10" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="K10" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="D11" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="E11" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="F11" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="G11" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="H11" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="G11" s="24">
+      <c r="I11" s="21">
         <v>10</v>
       </c>
-      <c r="H11" s="24">
+      <c r="J11" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="K11" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="D12" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="E12" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="F12" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="G12" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="H12" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="G12" s="24">
+      <c r="I12" s="21">
         <v>10</v>
       </c>
-      <c r="H12" s="24">
+      <c r="J12" s="21">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="K12" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="E13" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="F13" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="G13" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="H13" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="G13" s="24">
+      <c r="I13" s="21">
         <v>10</v>
       </c>
-      <c r="H13" s="24">
+      <c r="J13" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="K13" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="E14" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="F14" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="G14" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="H14" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="G14" s="24">
+      <c r="I14" s="21">
         <v>10</v>
       </c>
-      <c r="H14" s="24">
+      <c r="J14" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="K14" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="E15" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="F15" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="G15" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="H15" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="G15" s="24">
+      <c r="I15" s="21">
         <v>10</v>
       </c>
-      <c r="H15" s="24">
+      <c r="J15" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="K15" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="E16" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="F16" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="G16" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="H16" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="G16" s="24">
+      <c r="I16" s="21">
         <v>7</v>
       </c>
-      <c r="H16" s="24">
+      <c r="J16" s="21">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="K16" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="E17" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="F17" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="G17" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="H17" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="G17" s="24">
+      <c r="I17" s="21">
         <v>10</v>
       </c>
-      <c r="H17" s="24">
+      <c r="J17" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="K17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="D18" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="E18" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="F18" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="G18" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="H18" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="G18" s="24">
+      <c r="I18" s="21">
         <v>6</v>
       </c>
-      <c r="H18" s="24">
+      <c r="J18" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="K18" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="D19" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="E19" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="F19" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="G19" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="H19" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="G19" s="24">
+      <c r="I19" s="21">
         <v>10</v>
       </c>
-      <c r="H19" s="24">
+      <c r="J19" s="21">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="K19" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="D20" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="E20" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="F20" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="G20" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="H20" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="G20" s="24">
+      <c r="I20" s="21">
         <v>10</v>
       </c>
-      <c r="H20" s="24">
+      <c r="J20" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="K20" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="D21" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="E21" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="F21" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="G21" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="H21" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="G21" s="24">
+      <c r="I21" s="21">
         <v>3</v>
       </c>
-      <c r="H21" s="24">
+      <c r="J21" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="K21" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="D22" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="E22" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="F22" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="G22" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="H22" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="G22" s="24">
+      <c r="I22" s="21">
         <v>1</v>
       </c>
-      <c r="H22" s="24">
+      <c r="J22" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="K22" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="D23" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="E23" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="F23" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="G23" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="H23" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="G23" s="24">
+      <c r="I23" s="21">
         <v>6</v>
       </c>
-      <c r="H23" s="24">
+      <c r="J23" s="21">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="K23" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="D24" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="E24" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="F24" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="G24" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="H24" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="G24" s="24">
+      <c r="I24" s="21">
         <v>10</v>
       </c>
-      <c r="H24" s="24">
+      <c r="J24" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="K24" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="D25" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="E25" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="F25" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="G25" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="H25" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="G25" s="24">
+      <c r="I25" s="21">
         <v>10</v>
       </c>
-      <c r="H25" s="24">
+      <c r="J25" s="21">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="K25" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="D26" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="E26" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="F26" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="G26" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="H26" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="G26" s="24">
-        <v>0</v>
-      </c>
-      <c r="H26" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="D27" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="E27" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="F27" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="G27" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="H27" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="G27" s="24">
+      <c r="I27" s="21">
         <v>5</v>
       </c>
-      <c r="H27" s="24">
+      <c r="J27" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="K27" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="D28" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="E28" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="F28" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="G28" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="H28" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="G28" s="24">
+      <c r="I28" s="21">
         <v>1</v>
       </c>
-      <c r="H28" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="J28" s="21">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="D29" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="E29" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="F29" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="G29" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="H29" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="G29" s="24">
-        <v>0</v>
-      </c>
-      <c r="H29" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="I29" s="21">
+        <v>0</v>
+      </c>
+      <c r="J29" s="21">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="D30" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="E30" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="F30" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="G30" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="H30" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="G30" s="24">
+      <c r="I30" s="21">
         <v>4</v>
       </c>
-      <c r="H30" s="24">
+      <c r="J30" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="K30" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="D31" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="E31" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="F31" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="G31" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="H31" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="G31" s="24">
+      <c r="I31" s="21">
         <v>1</v>
       </c>
-      <c r="H31" s="24">
+      <c r="J31" s="21">
         <v>1</v>
       </c>
+      <c r="K31" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:H1048576 I1">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="A1:B1 I1:J1048576 K6:K31">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2364,16 +2777,36 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I1:J1048576 K6:K31 A1:B1">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="10"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:L1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>K1="No"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>K1="Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="G20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2388,16 +2821,16 @@
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
@@ -3486,7 +3919,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="3">
+        <f>COUNTIF(J3:J32,"&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="K33" s="3">
+        <f>COUNTIF(K3:K32,"&gt;0")</f>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A2:K32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="D1:F1"/>
@@ -3532,10 +3976,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -3601,10 +4045,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
@@ -3626,19 +4070,19 @@
         <v>175</v>
       </c>
       <c r="B10" s="10">
-        <f>COUNTIF('Errors (multiple)'!G2:G31, "&gt;0")</f>
+        <f>COUNTIF('Errors (multiple)'!I2:I31, "&gt;0")</f>
         <v>28</v>
       </c>
       <c r="C10" s="14">
-        <f>SUM('Errors (multiple)'!G2:G31)/10</f>
+        <f>SUM('Errors (multiple)'!I2:I31)/10</f>
         <v>19.7</v>
       </c>
       <c r="D10" s="15">
-        <f>SUM('Errors (multiple)'!H2:H31)/10</f>
+        <f>SUM('Errors (multiple)'!J2:J31)/10</f>
         <v>17.2</v>
       </c>
       <c r="E10" s="12">
-        <f>COUNTIF('Errors (multiple)'!G2:G31, "=0")</f>
+        <f>COUNTIF('Errors (multiple)'!I2:I31, "=0")</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>